<commit_message>
Updated income field names
</commit_message>
<xml_diff>
--- a/processing/Field name mapping.xlsx
+++ b/processing/Field name mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Housing\OrganizedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\my documents\Housing\processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -905,45 +905,15 @@
     <t>asset_val</t>
   </si>
   <si>
-    <t>antic_inc</t>
-  </si>
-  <si>
-    <t>antic_inc_tot</t>
-  </si>
-  <si>
-    <t>asset_impute</t>
-  </si>
-  <si>
-    <t>asset_final</t>
-  </si>
-  <si>
     <t>inc_mbr_num</t>
   </si>
   <si>
     <t>inc_code</t>
   </si>
   <si>
-    <t>inc_year</t>
-  </si>
-  <si>
     <t>inc_excl</t>
   </si>
   <si>
-    <t>inc_fin</t>
-  </si>
-  <si>
-    <t>inc_year_tot</t>
-  </si>
-  <si>
-    <t>inc_fin_tot</t>
-  </si>
-  <si>
-    <t>inc_tot</t>
-  </si>
-  <si>
-    <t>inc_deduct</t>
-  </si>
-  <si>
     <t>inc_adj</t>
   </si>
   <si>
@@ -1118,9 +1088,6 @@
     <t>v9</t>
   </si>
   <si>
-    <t>asset_tot</t>
-  </si>
-  <si>
     <t>Certification.Unique.ID.-.SHA.Field</t>
   </si>
   <si>
@@ -1446,6 +1413,39 @@
   </si>
   <si>
     <t>vouch_type</t>
+  </si>
+  <si>
+    <t>hh_inc_tot</t>
+  </si>
+  <si>
+    <t>hh_inc_adj</t>
+  </si>
+  <si>
+    <t>hh_inc_deduct</t>
+  </si>
+  <si>
+    <t>hh_inc_tot_adj</t>
+  </si>
+  <si>
+    <t>hh_asset_impute</t>
+  </si>
+  <si>
+    <t>asset_inc</t>
+  </si>
+  <si>
+    <t>hh_asset_inc</t>
+  </si>
+  <si>
+    <t>hh_asset_val</t>
+  </si>
+  <si>
+    <t>hh_asset_inc_final</t>
+  </si>
+  <si>
+    <t>hh_inc</t>
+  </si>
+  <si>
+    <t>inc</t>
   </si>
 </sst>
 </file>
@@ -1774,15 +1774,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="33.28515625" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -1790,25 +1790,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="B1" t="s">
         <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="E1" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="F1" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="G1" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="H1" t="s">
         <v>195</v>
@@ -1848,7 +1848,7 @@
         <v>236</v>
       </c>
       <c r="G3" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="H3" t="s">
         <v>199</v>
@@ -1859,7 +1859,7 @@
         <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="H4" t="s">
         <v>199</v>
@@ -1882,7 +1882,7 @@
         <v>237</v>
       </c>
       <c r="G5" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="H5" t="s">
         <v>198</v>
@@ -1893,7 +1893,7 @@
         <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="H6" t="s">
         <v>198</v>
@@ -1983,7 +1983,7 @@
         <v>241</v>
       </c>
       <c r="H12" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>243</v>
       </c>
       <c r="H15" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>149</v>
       </c>
       <c r="D30" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="H30" t="s">
         <v>213</v>
@@ -2321,7 +2321,7 @@
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2546,10 +2546,10 @@
         <v>185</v>
       </c>
       <c r="D46" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="H46" t="s">
-        <v>293</v>
+        <v>468</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2560,7 +2560,7 @@
         <v>39</v>
       </c>
       <c r="H47" t="s">
-        <v>364</v>
+        <v>470</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>17</v>
       </c>
       <c r="H48" t="s">
-        <v>294</v>
+        <v>469</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>18</v>
       </c>
       <c r="H49" t="s">
-        <v>295</v>
+        <v>467</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
         <v>19</v>
       </c>
       <c r="H50" t="s">
-        <v>296</v>
+        <v>471</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>179</v>
       </c>
       <c r="H51" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2615,10 +2615,10 @@
         <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="H52" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2635,7 +2635,7 @@
         <v>167</v>
       </c>
       <c r="H53" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2652,7 +2652,7 @@
         <v>169</v>
       </c>
       <c r="H54" t="s">
-        <v>299</v>
+        <v>473</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>170</v>
       </c>
       <c r="H55" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
         <v>171</v>
       </c>
       <c r="H56" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2700,7 +2700,7 @@
         <v>90</v>
       </c>
       <c r="H57" t="s">
-        <v>302</v>
+        <v>472</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
         <v>20</v>
       </c>
       <c r="H58" t="s">
-        <v>303</v>
+        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
         <v>21</v>
       </c>
       <c r="H59" t="s">
-        <v>304</v>
+        <v>463</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2745,7 +2745,7 @@
         <v>38</v>
       </c>
       <c r="H60" t="s">
-        <v>305</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2762,7 +2762,7 @@
         <v>22</v>
       </c>
       <c r="H61" t="s">
-        <v>306</v>
+        <v>466</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2779,10 +2779,10 @@
         <v>23</v>
       </c>
       <c r="F62" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="H62" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2799,10 +2799,10 @@
         <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="H63" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2819,10 +2819,10 @@
         <v>25</v>
       </c>
       <c r="F64" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="H64" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2836,10 +2836,10 @@
         <v>76</v>
       </c>
       <c r="F65" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="H65" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2853,10 +2853,10 @@
         <v>77</v>
       </c>
       <c r="F66" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="H66" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2873,10 +2873,10 @@
         <v>27</v>
       </c>
       <c r="F67" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="H67" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2893,10 +2893,10 @@
         <v>28</v>
       </c>
       <c r="F68" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="H68" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2913,10 +2913,10 @@
         <v>29</v>
       </c>
       <c r="F69" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="H69" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2933,10 +2933,10 @@
         <v>30</v>
       </c>
       <c r="F70" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="H70" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2953,10 +2953,10 @@
         <v>31</v>
       </c>
       <c r="F71" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="H71" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2973,10 +2973,10 @@
         <v>32</v>
       </c>
       <c r="F72" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="H72" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2993,10 +2993,10 @@
         <v>26</v>
       </c>
       <c r="F73" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="H73" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3013,10 +3013,10 @@
         <v>33</v>
       </c>
       <c r="F74" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="H74" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3033,10 +3033,10 @@
         <v>34</v>
       </c>
       <c r="F75" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="H75" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3053,10 +3053,10 @@
         <v>35</v>
       </c>
       <c r="F76" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="H76" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3073,10 +3073,10 @@
         <v>36</v>
       </c>
       <c r="F77" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="H77" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3093,10 +3093,10 @@
         <v>37</v>
       </c>
       <c r="F78" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="H78" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3107,7 +3107,7 @@
         <v>60</v>
       </c>
       <c r="C79" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -3141,7 +3141,7 @@
         <v>61</v>
       </c>
       <c r="C81" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D81" t="s">
         <v>8</v>
@@ -3161,7 +3161,7 @@
         <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="D82" t="s">
         <v>9</v>
@@ -3181,7 +3181,7 @@
         <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
@@ -3190,7 +3190,7 @@
         <v>206</v>
       </c>
       <c r="G83" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="H83" t="s">
         <v>206</v>
@@ -3198,32 +3198,32 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="H84" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="H85" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="B86" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C86" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="H86" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3292,10 +3292,10 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C92" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="H92" t="s">
         <v>194</v>
@@ -3326,7 +3326,7 @@
         <v>54</v>
       </c>
       <c r="F94" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="H94" t="s">
         <v>196</v>
@@ -3334,13 +3334,13 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D95" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="E95" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="H95" t="s">
         <v>196</v>
@@ -3356,17 +3356,17 @@
         <v>270</v>
       </c>
       <c r="H96" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="H97" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -3374,18 +3374,18 @@
         <v>1</v>
       </c>
       <c r="G98" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="H98" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="H99" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
@@ -3393,15 +3393,15 @@
         <v>2</v>
       </c>
       <c r="H100" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="H101" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>269</v>
       </c>
       <c r="H102" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -3422,114 +3422,114 @@
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G104" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="H104" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D105" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="H105" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="E106" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="F106" t="s">
         <v>238</v>
       </c>
       <c r="G106" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="H106" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="H107" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="H108" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="E109" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="F109" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="H109" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D110" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="E110" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="H110" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="H111" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="H112" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="H113" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="H114" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.25">
@@ -3537,308 +3537,308 @@
         <v>271</v>
       </c>
       <c r="H115" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.25">
       <c r="F116" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="H116" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="D117" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="E117" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="F117" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="H117" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="H118" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="D119" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="F119" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="H119" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="H120" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="D121" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="E121" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="F121" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="H121" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D122" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="H122" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="H123" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="H124" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="H125" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="H126" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="H127" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="H128" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="129" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="H129" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="130" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="H130" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="131" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="H131" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="132" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="H132" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="133" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="H133" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="134" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="H134" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="135" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="H135" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
     </row>
     <row r="136" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="H136" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="137" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="H137" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="138" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="H138" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="139" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="H139" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="140" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="H140" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="141" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="H141" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F142" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="H142" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
     </row>
     <row r="143" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F143" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="H143" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
     </row>
     <row r="144" spans="4:8" x14ac:dyDescent="0.25">
       <c r="F144" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="H144" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
     </row>
     <row r="145" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F145" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="H145" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
     </row>
     <row r="146" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F146" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="H146" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
     </row>
     <row r="147" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F147" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="H147" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="148" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F148" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="H148" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
     </row>
     <row r="149" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F149" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="H149" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
     </row>
     <row r="150" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F150" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="H150" t="s">
         <v>212</v>
@@ -3846,10 +3846,10 @@
     </row>
     <row r="151" spans="6:8" x14ac:dyDescent="0.25">
       <c r="G151" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="H151" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>